<commit_message>
update layout master barang pelanggan
</commit_message>
<xml_diff>
--- a/ImportExport/ExcelFiles/MasterBarangPelanggan.xlsx
+++ b/ImportExport/ExcelFiles/MasterBarangPelanggan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KERJA\AXATA\AxataPOSFilesResources\AxataPOSFilesResources\ImportExport\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2C3CCA-1349-494E-9203-B45F6417AC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FDFFAE-0480-4FBF-A324-B5815E37CCC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>NAMABARANG</t>
   </si>
@@ -84,9 +84,6 @@
     <t>PCS</t>
   </si>
   <si>
-    <t>1234KDFH</t>
-  </si>
-  <si>
     <t>HARGABELI</t>
   </si>
   <si>
@@ -112,6 +109,18 @@
   </si>
   <si>
     <t>SATUAN</t>
+  </si>
+  <si>
+    <t>BARCODE1</t>
+  </si>
+  <si>
+    <t>BARCODE2</t>
+  </si>
+  <si>
+    <t>BARCODE3</t>
+  </si>
+  <si>
+    <t>BARCODE4</t>
   </si>
 </sst>
 </file>
@@ -179,7 +188,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -191,9 +200,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,7 +479,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -489,7 +495,7 @@
     <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -497,10 +503,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -509,25 +515,25 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -555,17 +561,17 @@
       <c r="H2" s="1">
         <v>2000</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="1">
         <v>5000</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="1">
         <v>4000</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="1">
         <v>3000</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>17</v>
+      <c r="L2" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -593,17 +599,17 @@
       <c r="H3" s="1">
         <v>2000</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="1">
         <v>5000</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="1">
         <v>4000</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="1">
         <v>3000</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>17</v>
+      <c r="L3" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -631,17 +637,17 @@
       <c r="H4" s="1">
         <v>2000</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="1">
         <v>5000</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="1">
         <v>4000</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="1">
         <v>3000</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>17</v>
+      <c r="L4" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -669,17 +675,17 @@
       <c r="H5" s="1">
         <v>2000</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="1">
         <v>5000</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="1">
         <v>4000</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="1">
         <v>3000</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>17</v>
+      <c r="L5" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>